<commit_message>
Mise à jour dictionnaire de donnée
</commit_message>
<xml_diff>
--- a/2-Spécification, Analyse et conception/Dictionnaire_de_données_BDD_Supermarche.xlsx
+++ b/2-Spécification, Analyse et conception/Dictionnaire_de_données_BDD_Supermarche.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdel\Documents\GitHub\Projet_BDD_L3_MIAGE\2-Spécification, Analyse et conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E1DF5A-6018-4447-A632-F5244E0E883B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B65636-AB35-47C2-B93A-865CA5026574}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>Nom du client</t>
   </si>
   <si>
-    <t>VARCHAR2</t>
-  </si>
-  <si>
     <t>NOT NULL</t>
   </si>
   <si>
@@ -526,6 +523,9 @@
   </si>
   <si>
     <t>10, 2</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
   </si>
 </sst>
 </file>
@@ -895,12 +895,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I55" sqref="I55"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -990,58 +991,58 @@
         <v>13</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D4" s="13">
         <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="13.2">
       <c r="A5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D5" s="13">
         <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.2">
       <c r="A6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C6" s="11" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D6" s="13">
         <v>50</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.2">
       <c r="A7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="11" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D7" s="13">
         <v>10</v>
@@ -1049,91 +1050,91 @@
     </row>
     <row r="8" spans="1:26" ht="13.2">
       <c r="A8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D8" s="13">
         <v>25</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="26.4">
       <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D9" s="13">
         <v>5</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.2">
       <c r="A10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.2">
       <c r="A11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="26.4">
       <c r="A12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.2">
       <c r="A13" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1143,10 +1144,10 @@
     </row>
     <row r="14" spans="1:26" ht="13.2">
       <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -1161,30 +1162,30 @@
     </row>
     <row r="15" spans="1:26" ht="13.2">
       <c r="A15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D15" s="13">
         <v>50</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.2">
       <c r="A16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D16" s="13">
         <v>50</v>
@@ -1192,45 +1193,45 @@
     </row>
     <row r="17" spans="1:6" ht="13.2">
       <c r="A17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D17" s="13">
         <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.2">
       <c r="A18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C18" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="13"/>
       <c r="F18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.2">
       <c r="A19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D19" s="13">
         <v>20</v>
@@ -1238,7 +1239,7 @@
     </row>
     <row r="20" spans="1:6" ht="13.2">
       <c r="A20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1248,10 +1249,10 @@
     </row>
     <row r="21" spans="1:6" ht="13.2">
       <c r="A21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -1266,40 +1267,40 @@
     </row>
     <row r="22" spans="1:6" ht="39.6">
       <c r="A22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="13"/>
       <c r="F22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.2">
       <c r="A23" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>60</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.2">
       <c r="A24" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1309,10 +1310,10 @@
     </row>
     <row r="25" spans="1:6" ht="13.2">
       <c r="A25" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
@@ -1327,30 +1328,30 @@
     </row>
     <row r="26" spans="1:6" ht="13.2">
       <c r="A26" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>66</v>
-      </c>
       <c r="C26" s="11" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D26" s="13">
         <v>25</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.2">
       <c r="A27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="D27" s="13">
         <v>6.2</v>
@@ -1359,13 +1360,13 @@
     </row>
     <row r="28" spans="1:6" ht="13.2">
       <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D28" s="13">
         <v>75</v>
@@ -1373,139 +1374,139 @@
     </row>
     <row r="29" spans="1:6" ht="13.2">
       <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>73</v>
-      </c>
       <c r="C29" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="13">
         <v>5.2</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.2">
       <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="13" t="s">
+      <c r="F30" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.2">
       <c r="A31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="13">
         <v>5.2</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.2">
       <c r="A32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="13"/>
       <c r="F32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.2">
       <c r="A33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="13"/>
       <c r="F33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.2">
       <c r="A34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="13"/>
       <c r="F34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.2">
       <c r="A35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26.4">
       <c r="A36" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>91</v>
-      </c>
       <c r="C36" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.2">
       <c r="A37" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -1515,10 +1516,10 @@
     </row>
     <row r="38" spans="1:6" ht="13.2">
       <c r="A38" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>9</v>
@@ -1533,59 +1534,59 @@
     </row>
     <row r="39" spans="1:6" ht="13.2">
       <c r="A39" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D39" s="13">
         <v>25</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="13.2">
       <c r="A40" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D40" s="13">
         <v>75</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="26.4">
       <c r="A41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.2">
       <c r="A42" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -1595,10 +1596,10 @@
     </row>
     <row r="43" spans="1:6" ht="13.2">
       <c r="A43" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
@@ -1616,61 +1617,61 @@
         <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D44" s="13">
         <v>25</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="13.2">
       <c r="A45" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D45" s="13">
         <v>25</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="13.2">
       <c r="A46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D46" s="13">
         <v>50</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="13.2">
       <c r="A47" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D47" s="13">
         <v>10</v>
@@ -1678,13 +1679,13 @@
     </row>
     <row r="48" spans="1:6" ht="13.2">
       <c r="A48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="C48" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" s="13">
         <v>15.2</v>
@@ -1692,56 +1693,56 @@
     </row>
     <row r="49" spans="1:6" ht="29.4" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D49" s="13">
         <v>5</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13.2">
       <c r="A50" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="13.2">
       <c r="A51" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="13.2">
       <c r="A52" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
@@ -1751,10 +1752,10 @@
     </row>
     <row r="53" spans="1:6" ht="13.2">
       <c r="A53" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>9</v>
@@ -1769,30 +1770,30 @@
     </row>
     <row r="54" spans="1:6" ht="13.2">
       <c r="A54" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>120</v>
-      </c>
       <c r="C54" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D54" s="13">
         <v>25</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="13.2">
       <c r="A55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="C55" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D55" s="13">
         <v>75</v>
@@ -1800,7 +1801,7 @@
     </row>
     <row r="56" spans="1:6" ht="13.2">
       <c r="A56" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="7"/>
@@ -1810,10 +1811,10 @@
     </row>
     <row r="57" spans="1:6" ht="13.2">
       <c r="A57" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>9</v>
@@ -1828,47 +1829,47 @@
     </row>
     <row r="58" spans="1:6" ht="13.2">
       <c r="A58" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="11" t="s">
-        <v>127</v>
-      </c>
       <c r="C58" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D58" s="13">
         <v>25</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="13.2">
       <c r="A59" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D59" s="13">
         <v>50</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="13.2">
       <c r="A60" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D60" s="13">
         <v>10</v>
@@ -1876,13 +1877,13 @@
     </row>
     <row r="61" spans="1:6" ht="13.2">
       <c r="A61" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C61" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D61" s="13">
         <v>75</v>
@@ -1890,25 +1891,25 @@
     </row>
     <row r="62" spans="1:6" ht="13.2">
       <c r="A62" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="13.2">
       <c r="A63" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="16"/>
@@ -1918,10 +1919,10 @@
     </row>
     <row r="64" spans="1:6" ht="13.2">
       <c r="A64" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="19" t="s">
         <v>134</v>
-      </c>
-      <c r="B64" s="19" t="s">
-        <v>135</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>9</v>
@@ -1936,78 +1937,78 @@
     </row>
     <row r="65" spans="1:6" ht="13.2">
       <c r="A65" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="C65" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="D65" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="E65" s="19"/>
       <c r="F65" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="66">
       <c r="A66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>141</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D66" s="13">
         <v>30</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="13.2">
       <c r="A67" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="26.4">
       <c r="A68" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="13.2">
       <c r="A69" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="16"/>
@@ -2017,67 +2018,67 @@
     </row>
     <row r="70" spans="1:6" ht="26.4">
       <c r="A70" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B70" s="19" t="s">
-        <v>149</v>
-      </c>
       <c r="C70" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F70" s="11" t="s">
         <v>150</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="26.4">
       <c r="A71" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B71" s="19" t="s">
-        <v>153</v>
-      </c>
       <c r="C71" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F71" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="26.4">
       <c r="A72" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="C72" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D72" s="13"/>
       <c r="F72" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="26.4">
       <c r="A73" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="C73" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="13.2">
@@ -4869,5 +4870,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout sequence table sql et modif dictionnaire
</commit_message>
<xml_diff>
--- a/2-Spécification, Analyse et conception/Dictionnaire_de_données_BDD_Supermarche.xlsx
+++ b/2-Spécification, Analyse et conception/Dictionnaire_de_données_BDD_Supermarche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdel\Documents\GitHub\Projet_BDD_L3_MIAGE\2-Spécification, Analyse et conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B65636-AB35-47C2-B93A-865CA5026574}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB809E8-1D93-49B0-80FF-AD70E5DFB2C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="160">
   <si>
     <t>Table/Attribut</t>
   </si>
@@ -102,10 +102,6 @@
   <si>
     <t>Genre du client (sexe) 
 Homme, Femme, autre</t>
-  </si>
-  <si>
-    <t>CHECK IN "Homme", "Femme",
- "Autre"</t>
   </si>
   <si>
     <t>dateNaissance</t>
@@ -255,16 +251,7 @@
     <t>1, 3</t>
   </si>
   <si>
-    <t>CHECK IN "0.055" "0.20"</t>
-  </si>
-  <si>
     <t>prixTTC</t>
-  </si>
-  <si>
-    <t>Prix toute taxe comprise</t>
-  </si>
-  <si>
-    <t>PRIXHT + (PRIXHT * TAUXTVA)</t>
   </si>
   <si>
     <t>stock</t>
@@ -364,10 +351,6 @@
   <si>
     <t>Genre de l'employé (sexe)
 Homme, Femme, Autre</t>
-  </si>
-  <si>
-    <t>CHECK IN "Homme", "Femme",
- "Autre"</t>
   </si>
   <si>
     <t>Date de naissance de l'employé</t>
@@ -458,74 +441,86 @@
 ,"Annulé"</t>
   </si>
   <si>
-    <t>CHECK IN "En attente de traitement",
+    <t>Identifiant du client de la commande</t>
+  </si>
+  <si>
+    <t>#idEmploye</t>
+  </si>
+  <si>
+    <t>Identifiant de l'employé qui s'occupe 
+de la commande</t>
+  </si>
+  <si>
+    <t>Etrangere (Employe)</t>
+  </si>
+  <si>
+    <t>LigneDeCommande</t>
+  </si>
+  <si>
+    <t>#idProduit</t>
+  </si>
+  <si>
+    <t>Identifiant du produit de la
+ ligne de commande</t>
+  </si>
+  <si>
+    <t>Primaire
+Etrangere (Produit)</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY / FOREIGN KEY</t>
+  </si>
+  <si>
+    <t>#idCommande</t>
+  </si>
+  <si>
+    <t>Identifiant de la commande de la 
+ligne de commande</t>
+  </si>
+  <si>
+    <t>Primaire
+Etrangere (Commande)</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY / FOREIGN KEY</t>
+  </si>
+  <si>
+    <t>quantite</t>
+  </si>
+  <si>
+    <t>quantité de Produit de la ligne 
+de commande</t>
+  </si>
+  <si>
+    <t>prixVente</t>
+  </si>
+  <si>
+    <t>Prix de vente de la ligne de commande
+(quantité * produitTTC)</t>
+  </si>
+  <si>
+    <t>10, 2</t>
+  </si>
+  <si>
+    <t>VARCHAR2</t>
+  </si>
+  <si>
+    <t>Prix toute taxe comprise : PRIXHT + (PRIXHT * TAUXTVA)</t>
+  </si>
+  <si>
+    <t>CHECK (tauxTVA IN ("0.055" "0.20"))</t>
+  </si>
+  <si>
+    <t>CHECK ( genre IN ("Homme", "Femme","Autre"))</t>
+  </si>
+  <si>
+    <t>CHECK (genre IN ("Homme", "Femme","Autre"))</t>
+  </si>
+  <si>
+    <t>CHECK (statutCommande IN ("En attente de traitement",
 "En cours de traitement",
  "En attente de recuperation", "Livré"
-,"Annulé"</t>
-  </si>
-  <si>
-    <t>Identifiant du client de la commande</t>
-  </si>
-  <si>
-    <t>#idEmploye</t>
-  </si>
-  <si>
-    <t>Identifiant de l'employé qui s'occupe 
-de la commande</t>
-  </si>
-  <si>
-    <t>Etrangere (Employe)</t>
-  </si>
-  <si>
-    <t>LigneDeCommande</t>
-  </si>
-  <si>
-    <t>#idProduit</t>
-  </si>
-  <si>
-    <t>Identifiant du produit de la
- ligne de commande</t>
-  </si>
-  <si>
-    <t>Primaire
-Etrangere (Produit)</t>
-  </si>
-  <si>
-    <t>PRIMARY KEY / FOREIGN KEY</t>
-  </si>
-  <si>
-    <t>#idCommande</t>
-  </si>
-  <si>
-    <t>Identifiant de la commande de la 
-ligne de commande</t>
-  </si>
-  <si>
-    <t>Primaire
-Etrangere (Commande)</t>
-  </si>
-  <si>
-    <t>FOREIGN KEY / FOREIGN KEY</t>
-  </si>
-  <si>
-    <t>quantite</t>
-  </si>
-  <si>
-    <t>quantité de Produit de la ligne 
-de commande</t>
-  </si>
-  <si>
-    <t>prixVente</t>
-  </si>
-  <si>
-    <t>Prix de vente de la ligne de commande
-(quantité * produitTTC)</t>
-  </si>
-  <si>
-    <t>10, 2</t>
-  </si>
-  <si>
-    <t>VARCHAR</t>
+,"Annulé"))</t>
   </si>
 </sst>
 </file>
@@ -900,8 +895,8 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -991,7 +986,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D4" s="13">
         <v>25</v>
@@ -1008,7 +1003,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D5" s="13">
         <v>25</v>
@@ -1025,7 +1020,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D6" s="13">
         <v>50</v>
@@ -1042,7 +1037,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D7" s="13">
         <v>10</v>
@@ -1056,7 +1051,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D8" s="13">
         <v>25</v>
@@ -1073,68 +1068,68 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D9" s="13">
         <v>5</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.2">
       <c r="A10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.2">
       <c r="A11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="26.4">
       <c r="A12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.2">
       <c r="A13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1144,10 +1139,10 @@
     </row>
     <row r="14" spans="1:26" ht="13.2">
       <c r="A14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -1162,13 +1157,13 @@
     </row>
     <row r="15" spans="1:26" ht="13.2">
       <c r="A15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D15" s="13">
         <v>50</v>
@@ -1179,13 +1174,13 @@
     </row>
     <row r="16" spans="1:26" ht="13.2">
       <c r="A16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D16" s="13">
         <v>50</v>
@@ -1193,13 +1188,13 @@
     </row>
     <row r="17" spans="1:6" ht="13.2">
       <c r="A17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D17" s="13">
         <v>20</v>
@@ -1210,13 +1205,13 @@
     </row>
     <row r="18" spans="1:6" ht="13.2">
       <c r="A18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C18" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="13"/>
       <c r="F18" s="1" t="s">
@@ -1225,13 +1220,13 @@
     </row>
     <row r="19" spans="1:6" ht="13.2">
       <c r="A19" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D19" s="13">
         <v>20</v>
@@ -1239,7 +1234,7 @@
     </row>
     <row r="20" spans="1:6" ht="13.2">
       <c r="A20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1249,10 +1244,10 @@
     </row>
     <row r="21" spans="1:6" ht="13.2">
       <c r="A21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -1267,13 +1262,13 @@
     </row>
     <row r="22" spans="1:6" ht="39.6">
       <c r="A22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="13"/>
       <c r="F22" s="1" t="s">
@@ -1282,25 +1277,25 @@
     </row>
     <row r="23" spans="1:6" ht="13.2">
       <c r="A23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.2">
       <c r="A24" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1310,10 +1305,10 @@
     </row>
     <row r="25" spans="1:6" ht="13.2">
       <c r="A25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
@@ -1328,13 +1323,13 @@
     </row>
     <row r="26" spans="1:6" ht="13.2">
       <c r="A26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>65</v>
-      </c>
       <c r="C26" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D26" s="13">
         <v>25</v>
@@ -1345,13 +1340,13 @@
     </row>
     <row r="27" spans="1:6" ht="13.2">
       <c r="A27" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="D27" s="13">
         <v>6.2</v>
@@ -1360,13 +1355,13 @@
     </row>
     <row r="28" spans="1:6" ht="13.2">
       <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D28" s="13">
         <v>75</v>
@@ -1374,13 +1369,13 @@
     </row>
     <row r="29" spans="1:6" ht="13.2">
       <c r="A29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="C29" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="13">
         <v>5.2</v>
@@ -1391,47 +1386,45 @@
     </row>
     <row r="30" spans="1:6" ht="13.2">
       <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="13" t="s">
+      <c r="F30" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="26.4">
+      <c r="A31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="13.2">
-      <c r="A31" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="13">
         <v>5.2</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>79</v>
-      </c>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="13.2">
       <c r="A32" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="13"/>
       <c r="F32" s="1" t="s">
@@ -1440,13 +1433,13 @@
     </row>
     <row r="33" spans="1:6" ht="13.2">
       <c r="A33" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="13"/>
       <c r="F33" s="1" t="s">
@@ -1455,13 +1448,13 @@
     </row>
     <row r="34" spans="1:6" ht="13.2">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="13"/>
       <c r="F34" s="1" t="s">
@@ -1470,43 +1463,43 @@
     </row>
     <row r="35" spans="1:6" ht="13.2">
       <c r="A35" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26.4">
       <c r="A36" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.2">
       <c r="A37" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -1516,10 +1509,10 @@
     </row>
     <row r="38" spans="1:6" ht="13.2">
       <c r="A38" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>9</v>
@@ -1534,13 +1527,13 @@
     </row>
     <row r="39" spans="1:6" ht="13.2">
       <c r="A39" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D39" s="13">
         <v>25</v>
@@ -1551,13 +1544,13 @@
     </row>
     <row r="40" spans="1:6" ht="13.2">
       <c r="A40" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D40" s="13">
         <v>75</v>
@@ -1568,25 +1561,25 @@
     </row>
     <row r="41" spans="1:6" ht="26.4">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.2">
       <c r="A42" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -1596,10 +1589,10 @@
     </row>
     <row r="43" spans="1:6" ht="13.2">
       <c r="A43" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
@@ -1617,10 +1610,10 @@
         <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D44" s="13">
         <v>25</v>
@@ -1634,10 +1627,10 @@
         <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D45" s="13">
         <v>25</v>
@@ -1651,10 +1644,10 @@
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D46" s="13">
         <v>50</v>
@@ -1668,10 +1661,10 @@
         <v>20</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D47" s="13">
         <v>10</v>
@@ -1679,13 +1672,13 @@
     </row>
     <row r="48" spans="1:6" ht="13.2">
       <c r="A48" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" s="13">
         <v>15.2</v>
@@ -1696,53 +1689,53 @@
         <v>25</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D49" s="13">
         <v>5</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13.2">
       <c r="A50" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="13.2">
       <c r="A51" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="13.2">
       <c r="A52" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
@@ -1752,10 +1745,10 @@
     </row>
     <row r="53" spans="1:6" ht="13.2">
       <c r="A53" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>9</v>
@@ -1770,13 +1763,13 @@
     </row>
     <row r="54" spans="1:6" ht="13.2">
       <c r="A54" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D54" s="13">
         <v>25</v>
@@ -1787,13 +1780,13 @@
     </row>
     <row r="55" spans="1:6" ht="13.2">
       <c r="A55" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D55" s="13">
         <v>75</v>
@@ -1801,7 +1794,7 @@
     </row>
     <row r="56" spans="1:6" ht="13.2">
       <c r="A56" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="7"/>
@@ -1811,10 +1804,10 @@
     </row>
     <row r="57" spans="1:6" ht="13.2">
       <c r="A57" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>9</v>
@@ -1829,13 +1822,13 @@
     </row>
     <row r="58" spans="1:6" ht="13.2">
       <c r="A58" s="12" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D58" s="13">
         <v>25</v>
@@ -1849,10 +1842,10 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D59" s="13">
         <v>50</v>
@@ -1866,10 +1859,10 @@
         <v>20</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D60" s="13">
         <v>10</v>
@@ -1877,13 +1870,13 @@
     </row>
     <row r="61" spans="1:6" ht="13.2">
       <c r="A61" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D61" s="13">
         <v>75</v>
@@ -1891,25 +1884,25 @@
     </row>
     <row r="62" spans="1:6" ht="13.2">
       <c r="A62" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="13.2">
       <c r="A63" s="15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="16"/>
@@ -1919,10 +1912,10 @@
     </row>
     <row r="64" spans="1:6" ht="13.2">
       <c r="A64" s="18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>9</v>
@@ -1937,16 +1930,16 @@
     </row>
     <row r="65" spans="1:6" ht="13.2">
       <c r="A65" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E65" s="19"/>
       <c r="F65" s="1" t="s">
@@ -1955,60 +1948,60 @@
     </row>
     <row r="66" spans="1:6" ht="66">
       <c r="A66" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D66" s="13">
         <v>30</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="13.2">
       <c r="A67" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="26.4">
       <c r="A68" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="13.2">
       <c r="A69" s="15" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="16"/>
@@ -2018,49 +2011,49 @@
     </row>
     <row r="70" spans="1:6" ht="26.4">
       <c r="A70" s="18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="11" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="26.4">
       <c r="A71" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="19" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="26.4">
       <c r="A72" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D72" s="13"/>
       <c r="F72" s="1" t="s">
@@ -2069,16 +2062,16 @@
     </row>
     <row r="73" spans="1:6" ht="26.4">
       <c r="A73" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="13.2">

</xml_diff>